<commit_message>
Added patterns for DLPLIGHTCRAFTER
Smaller stuctured light patterns to match the smaller resolution of this TI projector, same sequence and settings should be used.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/BOM/ZooidReceiver.xlsx
+++ b/Hardware/PCB/BOM/ZooidReceiver.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>Designator</t>
   </si>
@@ -294,12 +294,21 @@
   </si>
   <si>
     <t>887-1462-1-ND</t>
+  </si>
+  <si>
+    <t>A24-HASM-450-ND</t>
+  </si>
+  <si>
+    <t>888-A24-HASM-450</t>
+  </si>
+  <si>
+    <t>Antenna 2.4GHZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -341,13 +350,16 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G27" totalsRowShown="0">
-  <autoFilter ref="A1:G27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G28" totalsRowShown="0">
+  <autoFilter ref="A1:G28"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Designator"/>
     <tableColumn id="2" name="Quantity"/>
@@ -624,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1255,8 +1267,29 @@
         <v>88</v>
       </c>
     </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>